<commit_message>
Cmabios, pruebas y otros
</commit_message>
<xml_diff>
--- a/models/ATT2ITM/restaurants/gijon/cbbd3295dd86f95883cab83c68e14003/att_text.xlsx
+++ b/models/ATT2ITM/restaurants/gijon/cbbd3295dd86f95883cab83c68e14003/att_text.xlsx
@@ -466,22 +466,22 @@
     <t>El Recetario</t>
   </si>
   <si>
-    <t>querer</t>
-  </si>
-  <si>
-    <t>arroz</t>
+    <t>estrella</t>
+  </si>
+  <si>
+    <t>michelin</t>
   </si>
   <si>
     <t>con</t>
   </si>
   <si>
-    <t>bogavante</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>nutella</t>
+    <t>vistas</t>
+  </si>
+  <si>
+    <t>al</t>
+  </si>
+  <si>
+    <t>mar</t>
   </si>
 </sst>
 </file>
@@ -893,22 +893,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.03139702975749969</v>
+        <v>-0.03359074890613556</v>
       </c>
       <c r="C3">
-        <v>-0.2275387048721313</v>
+        <v>-0.5196089148521423</v>
       </c>
       <c r="D3">
         <v>-0.01993044465780258</v>
       </c>
       <c r="E3">
-        <v>-0.6875299215316772</v>
+        <v>0.12701615691185</v>
       </c>
       <c r="F3">
-        <v>0.005951661616563797</v>
+        <v>-0.07536809146404266</v>
       </c>
       <c r="G3">
-        <v>-0.2768421173095703</v>
+        <v>0.809603750705719</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -916,22 +916,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.07358492910861969</v>
+        <v>-0.8167839646339417</v>
       </c>
       <c r="C4">
-        <v>-0.1738225221633911</v>
+        <v>-0.8884066939353943</v>
       </c>
       <c r="D4">
         <v>0.02816155552864075</v>
       </c>
       <c r="E4">
-        <v>-0.779805064201355</v>
+        <v>-0.8115954995155334</v>
       </c>
       <c r="F4">
-        <v>-0.05286424234509468</v>
+        <v>0.03218290582299232</v>
       </c>
       <c r="G4">
-        <v>-0.956321656703949</v>
+        <v>-0.599924623966217</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -939,22 +939,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1385040879249573</v>
+        <v>-0.1544578075408936</v>
       </c>
       <c r="C5">
-        <v>0.02761390618979931</v>
+        <v>-0.6413476467132568</v>
       </c>
       <c r="D5">
         <v>0.04703036323189735</v>
       </c>
       <c r="E5">
-        <v>-0.7166625261306763</v>
+        <v>0.4950044453144073</v>
       </c>
       <c r="F5">
-        <v>-0.007351307198405266</v>
+        <v>0.03352951258420944</v>
       </c>
       <c r="G5">
-        <v>-0.7375168204307556</v>
+        <v>0.2816846668720245</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -962,22 +962,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.1397248953580856</v>
+        <v>-0.1469646692276001</v>
       </c>
       <c r="C6">
-        <v>-0.5765587091445923</v>
+        <v>-0.6614106297492981</v>
       </c>
       <c r="D6">
         <v>-0.06201589107513428</v>
       </c>
       <c r="E6">
-        <v>-0.815290093421936</v>
+        <v>0.2909530103206635</v>
       </c>
       <c r="F6">
-        <v>-0.02759810909628868</v>
+        <v>0.03090273775160313</v>
       </c>
       <c r="G6">
-        <v>0.1494267880916595</v>
+        <v>-0.2271947413682938</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -985,22 +985,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.008724498562514782</v>
+        <v>-0.5598764419555664</v>
       </c>
       <c r="C7">
-        <v>0.3890273571014404</v>
+        <v>-0.8809182643890381</v>
       </c>
       <c r="D7">
         <v>0.02167757414281368</v>
       </c>
       <c r="E7">
-        <v>-0.3695134222507477</v>
+        <v>-0.9486192464828491</v>
       </c>
       <c r="F7">
-        <v>-0.03846596926450729</v>
+        <v>0.1126315221190453</v>
       </c>
       <c r="G7">
-        <v>-0.966922402381897</v>
+        <v>-0.9656290411949158</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1008,22 +1008,22 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.2308342903852463</v>
+        <v>-0.4402196705341339</v>
       </c>
       <c r="C8">
-        <v>0.04410717636346817</v>
+        <v>-0.7316592931747437</v>
       </c>
       <c r="D8">
         <v>-0.0670090988278389</v>
       </c>
       <c r="E8">
-        <v>0.5469337701797485</v>
+        <v>-0.9982599020004272</v>
       </c>
       <c r="F8">
-        <v>-0.02556062676012516</v>
+        <v>0.02982370369136333</v>
       </c>
       <c r="G8">
-        <v>-0.7377429008483887</v>
+        <v>-0.9704853892326355</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1031,22 +1031,22 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.1770470589399338</v>
+        <v>-0.04006646201014519</v>
       </c>
       <c r="C9">
-        <v>-0.3067018687725067</v>
+        <v>-0.4474335908889771</v>
       </c>
       <c r="D9">
         <v>0.1449004113674164</v>
       </c>
       <c r="E9">
-        <v>-0.9285509586334229</v>
+        <v>-0.9892990589141846</v>
       </c>
       <c r="F9">
-        <v>0.0440467968583107</v>
+        <v>-0.1344239264726639</v>
       </c>
       <c r="G9">
-        <v>-0.8104526400566101</v>
+        <v>-0.9913908839225769</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1054,22 +1054,22 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.04102562740445137</v>
+        <v>-0.678486704826355</v>
       </c>
       <c r="C10">
-        <v>-0.03156963363289833</v>
+        <v>-0.7848523855209351</v>
       </c>
       <c r="D10">
         <v>0.01730342768132687</v>
       </c>
       <c r="E10">
-        <v>0.1563464552164078</v>
+        <v>-0.5793465375900269</v>
       </c>
       <c r="F10">
-        <v>-0.007500860374420881</v>
+        <v>0.01794522441923618</v>
       </c>
       <c r="G10">
-        <v>-0.9795178771018982</v>
+        <v>-0.8501807451248169</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1077,22 +1077,22 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.08024173974990845</v>
+        <v>-0.2405839562416077</v>
       </c>
       <c r="C11">
-        <v>-0.138634666800499</v>
+        <v>-0.2491514533758163</v>
       </c>
       <c r="D11">
         <v>-0.01736254058778286</v>
       </c>
       <c r="E11">
-        <v>-0.9948744177818298</v>
+        <v>-0.05563816055655479</v>
       </c>
       <c r="F11">
-        <v>0.0181287731975317</v>
+        <v>0.03945749625563622</v>
       </c>
       <c r="G11">
-        <v>-0.9268853664398193</v>
+        <v>-0.896565854549408</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1100,22 +1100,22 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.1654161512851715</v>
+        <v>-0.08923926949501038</v>
       </c>
       <c r="C12">
-        <v>0.02166873402893543</v>
+        <v>-0.746213436126709</v>
       </c>
       <c r="D12">
         <v>0.02432528138160706</v>
       </c>
       <c r="E12">
-        <v>-0.1953023821115494</v>
+        <v>-0.9280543923377991</v>
       </c>
       <c r="F12">
-        <v>0.02937879040837288</v>
+        <v>-0.03975511342287064</v>
       </c>
       <c r="G12">
-        <v>-0.9164899587631226</v>
+        <v>-0.7724349498748779</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1123,22 +1123,22 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.2509841024875641</v>
+        <v>-0.860962986946106</v>
       </c>
       <c r="C13">
-        <v>-0.9421858787536621</v>
+        <v>-0.9974372386932373</v>
       </c>
       <c r="D13">
         <v>-0.04269621521234512</v>
       </c>
       <c r="E13">
-        <v>-0.9978458285331726</v>
+        <v>-0.6938214302062988</v>
       </c>
       <c r="F13">
-        <v>0.02465034462511539</v>
+        <v>0.002812066348269582</v>
       </c>
       <c r="G13">
-        <v>-0.6789498329162598</v>
+        <v>-0.3624206781387329</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1146,22 +1146,22 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.09046328067779541</v>
+        <v>-0.2722574472427368</v>
       </c>
       <c r="C14">
-        <v>-0.005254051648080349</v>
+        <v>-0.7817711234092712</v>
       </c>
       <c r="D14">
         <v>-0.05626948550343513</v>
       </c>
       <c r="E14">
-        <v>-0.04219901189208031</v>
+        <v>0.8885279297828674</v>
       </c>
       <c r="F14">
-        <v>-0.003996020182967186</v>
+        <v>-0.06073013693094254</v>
       </c>
       <c r="G14">
-        <v>-0.4733487367630005</v>
+        <v>0.855588972568512</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1169,22 +1169,22 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.2434754371643066</v>
+        <v>-0.3270552754402161</v>
       </c>
       <c r="C15">
-        <v>0.04145771265029907</v>
+        <v>-0.6949540972709656</v>
       </c>
       <c r="D15">
         <v>-0.0252371896058321</v>
       </c>
       <c r="E15">
-        <v>0.4732419848442078</v>
+        <v>-0.9983787536621094</v>
       </c>
       <c r="F15">
-        <v>-0.01929440721869469</v>
+        <v>-0.1111171171069145</v>
       </c>
       <c r="G15">
-        <v>-0.9564285278320312</v>
+        <v>-0.9944649338722229</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1192,22 +1192,22 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.1295372992753983</v>
+        <v>0.004822995979338884</v>
       </c>
       <c r="C16">
-        <v>-0.2909516096115112</v>
+        <v>-0.8739892840385437</v>
       </c>
       <c r="D16">
         <v>-0.02234870195388794</v>
       </c>
       <c r="E16">
-        <v>-0.9619632959365845</v>
+        <v>0.6932404041290283</v>
       </c>
       <c r="F16">
-        <v>0.03347219154238701</v>
+        <v>-0.008989329449832439</v>
       </c>
       <c r="G16">
-        <v>-0.5388504266738892</v>
+        <v>0.578779399394989</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1215,22 +1215,22 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.1048337519168854</v>
+        <v>-0.557221531867981</v>
       </c>
       <c r="C17">
-        <v>-0.6034061908721924</v>
+        <v>-0.9772185087203979</v>
       </c>
       <c r="D17">
         <v>-0.121358260512352</v>
       </c>
       <c r="E17">
-        <v>0.3271937668323517</v>
+        <v>-0.6236557364463806</v>
       </c>
       <c r="F17">
-        <v>0.007911341264843941</v>
+        <v>0.06096363067626953</v>
       </c>
       <c r="G17">
-        <v>-0.4041747450828552</v>
+        <v>-0.2963291108608246</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1238,22 +1238,22 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.1639518588781357</v>
+        <v>-0.03904044255614281</v>
       </c>
       <c r="C18">
-        <v>-0.1948477327823639</v>
+        <v>0.1072582751512527</v>
       </c>
       <c r="D18">
         <v>-0.04310474544763565</v>
       </c>
       <c r="E18">
-        <v>-0.8615569472312927</v>
+        <v>-0.560639500617981</v>
       </c>
       <c r="F18">
-        <v>-0.06158813461661339</v>
+        <v>-0.1177856549620628</v>
       </c>
       <c r="G18">
-        <v>-0.5652071833610535</v>
+        <v>-0.8637717366218567</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1261,22 +1261,22 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.1351955682039261</v>
+        <v>-0.2934398651123047</v>
       </c>
       <c r="C19">
-        <v>0.5815637707710266</v>
+        <v>-0.7730147838592529</v>
       </c>
       <c r="D19">
         <v>0.01265244465321302</v>
       </c>
       <c r="E19">
-        <v>0.8403233885765076</v>
+        <v>0.3954764604568481</v>
       </c>
       <c r="F19">
-        <v>-0.04117758572101593</v>
+        <v>0.07381105422973633</v>
       </c>
       <c r="G19">
-        <v>-0.9471027851104736</v>
+        <v>-0.7101958394050598</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1284,22 +1284,22 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-0.2215674370527267</v>
+        <v>0.8874918222427368</v>
       </c>
       <c r="C20">
-        <v>-0.6938214302062988</v>
+        <v>0.9811134934425354</v>
       </c>
       <c r="D20">
         <v>0.07948651164770126</v>
       </c>
       <c r="E20">
-        <v>-0.6247695088386536</v>
+        <v>0.538830041885376</v>
       </c>
       <c r="F20">
-        <v>-0.02084147743880749</v>
+        <v>0.1336827576160431</v>
       </c>
       <c r="G20">
-        <v>-0.636704683303833</v>
+        <v>0.9012847542762756</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1307,22 +1307,22 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.1330622434616089</v>
+        <v>-0.09268617630004883</v>
       </c>
       <c r="C21">
-        <v>-0.4017889201641083</v>
+        <v>-0.3530422449111938</v>
       </c>
       <c r="D21">
         <v>-0.1262119859457016</v>
       </c>
       <c r="E21">
-        <v>-0.2270063608884811</v>
+        <v>-0.9492899179458618</v>
       </c>
       <c r="F21">
-        <v>-0.05306074768304825</v>
+        <v>0.0827237069606781</v>
       </c>
       <c r="G21">
-        <v>-0.9553150534629822</v>
+        <v>0.1800378859043121</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1330,22 +1330,22 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.06428739428520203</v>
+        <v>-0.491210401058197</v>
       </c>
       <c r="C22">
-        <v>-0.3760586380958557</v>
+        <v>-0.8917205929756165</v>
       </c>
       <c r="D22">
         <v>-0.02642691694200039</v>
       </c>
       <c r="E22">
-        <v>-0.865586519241333</v>
+        <v>-0.8416656255722046</v>
       </c>
       <c r="F22">
-        <v>-0.008240004070103168</v>
+        <v>-0.03166976198554039</v>
       </c>
       <c r="G22">
-        <v>-0.9753626585006714</v>
+        <v>-0.9218674898147583</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1353,22 +1353,22 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.09565658867359161</v>
+        <v>-0.6701903939247131</v>
       </c>
       <c r="C23">
-        <v>-0.0007540357182733715</v>
+        <v>-0.8684900403022766</v>
       </c>
       <c r="D23">
         <v>0.08351524174213409</v>
       </c>
       <c r="E23">
-        <v>-0.4112256765365601</v>
+        <v>-0.3145613968372345</v>
       </c>
       <c r="F23">
-        <v>-0.001682665897533298</v>
+        <v>0.001965481787919998</v>
       </c>
       <c r="G23">
-        <v>-0.9526482820510864</v>
+        <v>-0.7547922730445862</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1376,22 +1376,22 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>-0.2367579787969589</v>
+        <v>-0.4197549223899841</v>
       </c>
       <c r="C24">
-        <v>-0.1465174704790115</v>
+        <v>-0.3779191076755524</v>
       </c>
       <c r="D24">
         <v>0.04450838267803192</v>
       </c>
       <c r="E24">
-        <v>0.4384564757347107</v>
+        <v>0.7951350808143616</v>
       </c>
       <c r="F24">
-        <v>-0.08599822968244553</v>
+        <v>-0.005462632980197668</v>
       </c>
       <c r="G24">
-        <v>-0.7577504515647888</v>
+        <v>0.7776064276695251</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1399,22 +1399,22 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.001605801051482558</v>
+        <v>0.1451413929462433</v>
       </c>
       <c r="C25">
-        <v>-0.05648710951209068</v>
+        <v>-0.7318607568740845</v>
       </c>
       <c r="D25">
         <v>0.04705847427248955</v>
       </c>
       <c r="E25">
-        <v>-0.3009950816631317</v>
+        <v>0.767476499080658</v>
       </c>
       <c r="F25">
-        <v>-0.03636303916573524</v>
+        <v>0.0180005244910717</v>
       </c>
       <c r="G25">
-        <v>-0.3252804577350616</v>
+        <v>-0.3387508392333984</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1422,22 +1422,22 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>-0.1103078871965408</v>
+        <v>0.5453510880470276</v>
       </c>
       <c r="C26">
-        <v>0.3776660561561584</v>
+        <v>-0.6903300881385803</v>
       </c>
       <c r="D26">
         <v>0.02250096015632153</v>
       </c>
       <c r="E26">
-        <v>0.5536143183708191</v>
+        <v>-0.9846396446228027</v>
       </c>
       <c r="F26">
-        <v>-0.0617864727973938</v>
+        <v>-0.1011494621634483</v>
       </c>
       <c r="G26">
-        <v>-0.9996651411056519</v>
+        <v>-0.9853723645210266</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1445,22 +1445,22 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-0.1827327907085419</v>
+        <v>0.1619611233472824</v>
       </c>
       <c r="C27">
-        <v>-0.7594412565231323</v>
+        <v>-0.6594720482826233</v>
       </c>
       <c r="D27">
         <v>-0.1233849674463272</v>
       </c>
       <c r="E27">
-        <v>-0.9450672268867493</v>
+        <v>-0.6030306816101074</v>
       </c>
       <c r="F27">
-        <v>0.02083835378289223</v>
+        <v>-0.01343252044171095</v>
       </c>
       <c r="G27">
-        <v>-0.6178966164588928</v>
+        <v>-0.6772040128707886</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1468,22 +1468,22 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-0.3162509500980377</v>
+        <v>-0.109937995672226</v>
       </c>
       <c r="C28">
-        <v>-0.8398565649986267</v>
+        <v>-0.7569367289543152</v>
       </c>
       <c r="D28">
         <v>-0.06818854063749313</v>
       </c>
       <c r="E28">
-        <v>-0.7696508765220642</v>
+        <v>0.7667010426521301</v>
       </c>
       <c r="F28">
-        <v>-0.04189478233456612</v>
+        <v>0.2510153949260712</v>
       </c>
       <c r="G28">
-        <v>-0.8565574884414673</v>
+        <v>0.2265793532133102</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1491,22 +1491,22 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.2041187584400177</v>
+        <v>-0.3958983719348907</v>
       </c>
       <c r="C29">
-        <v>0.2516311705112457</v>
+        <v>-0.9392398595809937</v>
       </c>
       <c r="D29">
         <v>-0.03994195908308029</v>
       </c>
       <c r="E29">
-        <v>0.2884308397769928</v>
+        <v>-0.4826931059360504</v>
       </c>
       <c r="F29">
-        <v>-0.01498268358409405</v>
+        <v>0.08885098248720169</v>
       </c>
       <c r="G29">
-        <v>-0.2008350938558578</v>
+        <v>0.3559498190879822</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1514,22 +1514,22 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>-0.1130897402763367</v>
+        <v>-0.2554159164428711</v>
       </c>
       <c r="C30">
-        <v>-0.2190470099449158</v>
+        <v>-0.8645114302635193</v>
       </c>
       <c r="D30">
         <v>0.0606522224843502</v>
       </c>
       <c r="E30">
-        <v>-0.8733999729156494</v>
+        <v>-0.7130152583122253</v>
       </c>
       <c r="F30">
-        <v>-0.06554839760065079</v>
+        <v>0.07962468266487122</v>
       </c>
       <c r="G30">
-        <v>-0.8386262655258179</v>
+        <v>-0.5115605592727661</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1537,22 +1537,22 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.1957163959741592</v>
+        <v>-0.04629769921302795</v>
       </c>
       <c r="C31">
-        <v>0.3246498703956604</v>
+        <v>-0.6723551154136658</v>
       </c>
       <c r="D31">
         <v>0.06440075486898422</v>
       </c>
       <c r="E31">
-        <v>-0.7549882531166077</v>
+        <v>-0.866344690322876</v>
       </c>
       <c r="F31">
-        <v>-0.007313597481697798</v>
+        <v>0.1704156696796417</v>
       </c>
       <c r="G31">
-        <v>-0.9900133609771729</v>
+        <v>-0.800368070602417</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1560,22 +1560,22 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.1635313332080841</v>
+        <v>-0.2315698713064194</v>
       </c>
       <c r="C32">
-        <v>-0.007456767838448286</v>
+        <v>-0.617897629737854</v>
       </c>
       <c r="D32">
         <v>0.005352716892957687</v>
       </c>
       <c r="E32">
-        <v>0.02365428395569324</v>
+        <v>-0.9907730221748352</v>
       </c>
       <c r="F32">
-        <v>0.02811170183122158</v>
+        <v>-0.05484180524945259</v>
       </c>
       <c r="G32">
-        <v>0.05359186232089996</v>
+        <v>-0.9145018458366394</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1583,22 +1583,22 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.1491803079843521</v>
+        <v>-0.5494901537895203</v>
       </c>
       <c r="C33">
-        <v>-0.8430277109146118</v>
+        <v>-0.7366059422492981</v>
       </c>
       <c r="D33">
         <v>-0.06796200573444366</v>
       </c>
       <c r="E33">
-        <v>-0.8706366419792175</v>
+        <v>-0.9758070707321167</v>
       </c>
       <c r="F33">
-        <v>0.01575702428817749</v>
+        <v>-0.04726274311542511</v>
       </c>
       <c r="G33">
-        <v>-0.9931868314743042</v>
+        <v>-0.371868371963501</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1606,22 +1606,22 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>-0.01834283582866192</v>
+        <v>0.7829055190086365</v>
       </c>
       <c r="C34">
-        <v>0.3866369724273682</v>
+        <v>0.8363088965415955</v>
       </c>
       <c r="D34">
         <v>0.1424376517534256</v>
       </c>
       <c r="E34">
-        <v>-0.7834450006484985</v>
+        <v>0.3220262229442596</v>
       </c>
       <c r="F34">
-        <v>-0.04653657972812653</v>
+        <v>0.0830705463886261</v>
       </c>
       <c r="G34">
-        <v>-0.7517844438552856</v>
+        <v>-0.8724210262298584</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1629,22 +1629,22 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.1622022092342377</v>
+        <v>-0.6334463953971863</v>
       </c>
       <c r="C35">
-        <v>0.2032144367694855</v>
+        <v>-0.7447785139083862</v>
       </c>
       <c r="D35">
         <v>0.02593592926859856</v>
       </c>
       <c r="E35">
-        <v>0.575157105922699</v>
+        <v>-0.85745769739151</v>
       </c>
       <c r="F35">
-        <v>-0.001068441662937403</v>
+        <v>-0.07780510187149048</v>
       </c>
       <c r="G35">
-        <v>-0.6752426028251648</v>
+        <v>-0.8660248517990112</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1652,22 +1652,22 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.01916348747909069</v>
+        <v>-0.2723492980003357</v>
       </c>
       <c r="C36">
-        <v>-0.684205949306488</v>
+        <v>-0.5318648815155029</v>
       </c>
       <c r="D36">
         <v>0.06191781535744667</v>
       </c>
       <c r="E36">
-        <v>-0.9763004183769226</v>
+        <v>-0.995384156703949</v>
       </c>
       <c r="F36">
-        <v>0.03254967555403709</v>
+        <v>-0.1162090077996254</v>
       </c>
       <c r="G36">
-        <v>-0.7103041410446167</v>
+        <v>-0.94512540102005</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1675,22 +1675,22 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>-0.2099777907133102</v>
+        <v>-0.4999088644981384</v>
       </c>
       <c r="C37">
-        <v>-0.7160322666168213</v>
+        <v>-0.4477615356445312</v>
       </c>
       <c r="D37">
         <v>-0.02667593955993652</v>
       </c>
       <c r="E37">
-        <v>-0.9680235981941223</v>
+        <v>-0.7638223767280579</v>
       </c>
       <c r="F37">
-        <v>0.01677332818508148</v>
+        <v>-0.1222119703888893</v>
       </c>
       <c r="G37">
-        <v>-0.9348804354667664</v>
+        <v>-0.9572077393531799</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1698,22 +1698,22 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.2615764737129211</v>
+        <v>-0.3842324316501617</v>
       </c>
       <c r="C38">
-        <v>0.1967136710882187</v>
+        <v>-0.7654815316200256</v>
       </c>
       <c r="D38">
         <v>0.03934511169791222</v>
       </c>
       <c r="E38">
-        <v>0.153408944606781</v>
+        <v>-0.8970401287078857</v>
       </c>
       <c r="F38">
-        <v>0.03288605436682701</v>
+        <v>0.1568013280630112</v>
       </c>
       <c r="G38">
-        <v>-0.147821232676506</v>
+        <v>-0.2645596563816071</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1721,22 +1721,22 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.1139286756515503</v>
+        <v>-0.7316830158233643</v>
       </c>
       <c r="C39">
-        <v>0.145730048418045</v>
+        <v>-0.8257516622543335</v>
       </c>
       <c r="D39">
         <v>-0.001279015094041824</v>
       </c>
       <c r="E39">
-        <v>0.2246523648500443</v>
+        <v>-0.8811835050582886</v>
       </c>
       <c r="F39">
-        <v>-0.03861869499087334</v>
+        <v>-0.2834503948688507</v>
       </c>
       <c r="G39">
-        <v>-0.7924364805221558</v>
+        <v>-0.9545806050300598</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1744,22 +1744,22 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>-0.02507902681827545</v>
+        <v>-0.4829432666301727</v>
       </c>
       <c r="C40">
-        <v>-0.1404051035642624</v>
+        <v>-0.9480764269828796</v>
       </c>
       <c r="D40">
         <v>0.009133749641478062</v>
       </c>
       <c r="E40">
-        <v>-0.1233215928077698</v>
+        <v>-0.4059863984584808</v>
       </c>
       <c r="F40">
-        <v>-0.04875855147838593</v>
+        <v>0.1291913688182831</v>
       </c>
       <c r="G40">
-        <v>-0.9257273077964783</v>
+        <v>-0.3890413641929626</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1767,22 +1767,22 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.1467921882867813</v>
+        <v>0.08029559999704361</v>
       </c>
       <c r="C41">
-        <v>-0.1221229806542397</v>
+        <v>-0.3958306610584259</v>
       </c>
       <c r="D41">
         <v>0.07560697197914124</v>
       </c>
       <c r="E41">
-        <v>-0.9329342246055603</v>
+        <v>-0.9430599808692932</v>
       </c>
       <c r="F41">
-        <v>0.03346563875675201</v>
+        <v>0.02727195993065834</v>
       </c>
       <c r="G41">
-        <v>-0.9969837069511414</v>
+        <v>-0.9666528701782227</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1790,22 +1790,22 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.04374710842967033</v>
+        <v>-0.2500399649143219</v>
       </c>
       <c r="C42">
-        <v>-0.2118294835090637</v>
+        <v>-0.7764544486999512</v>
       </c>
       <c r="D42">
         <v>-0.07043815404176712</v>
       </c>
       <c r="E42">
-        <v>-0.6563743948936462</v>
+        <v>-0.707601010799408</v>
       </c>
       <c r="F42">
-        <v>0.004579153843224049</v>
+        <v>-0.1016172394156456</v>
       </c>
       <c r="G42">
-        <v>0.09906049817800522</v>
+        <v>-0.6752422451972961</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1813,22 +1813,22 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.137325718998909</v>
+        <v>-0.4512624144554138</v>
       </c>
       <c r="C43">
-        <v>-0.3356703221797943</v>
+        <v>-0.8085687756538391</v>
       </c>
       <c r="D43">
         <v>0.04067666828632355</v>
       </c>
       <c r="E43">
-        <v>-0.9280392527580261</v>
+        <v>-0.6317565441131592</v>
       </c>
       <c r="F43">
-        <v>-0.01655725762248039</v>
+        <v>0.04340843111276627</v>
       </c>
       <c r="G43">
-        <v>-0.974235475063324</v>
+        <v>-0.3661302328109741</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1836,22 +1836,22 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>-0.01914928667247295</v>
+        <v>0.2433108240365982</v>
       </c>
       <c r="C44">
-        <v>-0.391999363899231</v>
+        <v>-0.7169533371925354</v>
       </c>
       <c r="D44">
         <v>-0.02925202809274197</v>
       </c>
       <c r="E44">
-        <v>-0.6142247319221497</v>
+        <v>-0.8026338219642639</v>
       </c>
       <c r="F44">
-        <v>-0.0272618755698204</v>
+        <v>0.02825219742953777</v>
       </c>
       <c r="G44">
-        <v>-0.5739508867263794</v>
+        <v>0.2900926470756531</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1859,22 +1859,22 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.03228273987770081</v>
+        <v>-0.3254137933254242</v>
       </c>
       <c r="C45">
-        <v>0.1271966099739075</v>
+        <v>-0.6828389167785645</v>
       </c>
       <c r="D45">
         <v>-0.007884754799306393</v>
       </c>
       <c r="E45">
-        <v>-0.5050836205482483</v>
+        <v>0.1730757802724838</v>
       </c>
       <c r="F45">
-        <v>-0.0314745120704174</v>
+        <v>0.002691746689379215</v>
       </c>
       <c r="G45">
-        <v>-0.2029300332069397</v>
+        <v>-0.4355600476264954</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1882,22 +1882,22 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>-0.2551748752593994</v>
+        <v>-0.4814819097518921</v>
       </c>
       <c r="C46">
-        <v>-0.6466405391693115</v>
+        <v>-0.8118525743484497</v>
       </c>
       <c r="D46">
         <v>0.003958413377404213</v>
       </c>
       <c r="E46">
-        <v>-0.5237076282501221</v>
+        <v>-0.9791237711906433</v>
       </c>
       <c r="F46">
-        <v>-0.03238817676901817</v>
+        <v>-0.01065017934888601</v>
       </c>
       <c r="G46">
-        <v>-0.9829084873199463</v>
+        <v>-0.978380024433136</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1905,22 +1905,22 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>-0.03248865529894829</v>
+        <v>-0.5510633587837219</v>
       </c>
       <c r="C47">
-        <v>-0.3059641718864441</v>
+        <v>-0.6827319264411926</v>
       </c>
       <c r="D47">
         <v>0.07034752517938614</v>
       </c>
       <c r="E47">
-        <v>-0.8155697584152222</v>
+        <v>0.8591399192810059</v>
       </c>
       <c r="F47">
-        <v>0.02416660264134407</v>
+        <v>0.08558908849954605</v>
       </c>
       <c r="G47">
-        <v>-0.8314567804336548</v>
+        <v>0.7275458574295044</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1928,22 +1928,22 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>-0.1519453972578049</v>
+        <v>-0.7944019436836243</v>
       </c>
       <c r="C48">
-        <v>-0.3123170733451843</v>
+        <v>-0.9906272888183594</v>
       </c>
       <c r="D48">
         <v>-0.03336049243807793</v>
       </c>
       <c r="E48">
-        <v>-0.9138671159744263</v>
+        <v>-0.9938090443611145</v>
       </c>
       <c r="F48">
-        <v>0.04007143527269363</v>
+        <v>-0.04697434976696968</v>
       </c>
       <c r="G48">
-        <v>-0.9915734529495239</v>
+        <v>-0.9908110499382019</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1951,22 +1951,22 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.1324503868818283</v>
+        <v>-0.1719983071088791</v>
       </c>
       <c r="C49">
-        <v>-0.2500065863132477</v>
+        <v>0.003618794493377209</v>
       </c>
       <c r="D49">
         <v>-0.03831911832094193</v>
       </c>
       <c r="E49">
-        <v>-0.919320285320282</v>
+        <v>-0.9642122387886047</v>
       </c>
       <c r="F49">
-        <v>-0.03216388821601868</v>
+        <v>0.003743630368262529</v>
       </c>
       <c r="G49">
-        <v>0.9393207430839539</v>
+        <v>-0.7565896511077881</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1974,22 +1974,22 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>-0.1244695261120796</v>
+        <v>-0.3454149067401886</v>
       </c>
       <c r="C50">
-        <v>-0.6516808271408081</v>
+        <v>-0.9473150372505188</v>
       </c>
       <c r="D50">
         <v>-0.05503276363015175</v>
       </c>
       <c r="E50">
-        <v>0.3059731125831604</v>
+        <v>0.7409615516662598</v>
       </c>
       <c r="F50">
-        <v>-0.06271106004714966</v>
+        <v>0.1704664826393127</v>
       </c>
       <c r="G50">
-        <v>-0.920156717300415</v>
+        <v>0.1307561844587326</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1997,22 +1997,22 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.1722747981548309</v>
+        <v>0.1710321754217148</v>
       </c>
       <c r="C51">
-        <v>0.9617406129837036</v>
+        <v>-0.8789467811584473</v>
       </c>
       <c r="D51">
         <v>0.194149523973465</v>
       </c>
       <c r="E51">
-        <v>0.9933235049247742</v>
+        <v>-0.9633303284645081</v>
       </c>
       <c r="F51">
-        <v>-0.01497944071888924</v>
+        <v>-0.00665891170501709</v>
       </c>
       <c r="G51">
-        <v>-0.5192955136299133</v>
+        <v>-0.5511583089828491</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2020,22 +2020,22 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.1089630052447319</v>
+        <v>-0.4341797828674316</v>
       </c>
       <c r="C52">
-        <v>0.3147250711917877</v>
+        <v>-0.9119647145271301</v>
       </c>
       <c r="D52">
         <v>0.03833673521876335</v>
       </c>
       <c r="E52">
-        <v>-0.7403443455696106</v>
+        <v>-0.9755855202674866</v>
       </c>
       <c r="F52">
-        <v>-0.03398719057440758</v>
+        <v>-0.02278884500265121</v>
       </c>
       <c r="G52">
-        <v>-0.7575714588165283</v>
+        <v>-0.781226634979248</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2043,22 +2043,22 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.1823897808790207</v>
+        <v>-0.7377780079841614</v>
       </c>
       <c r="C53">
-        <v>-0.06502455472946167</v>
+        <v>-0.8107254505157471</v>
       </c>
       <c r="D53">
         <v>0.2227922379970551</v>
       </c>
       <c r="E53">
-        <v>-0.9412976503372192</v>
+        <v>0.7539929151535034</v>
       </c>
       <c r="F53">
-        <v>-0.05448809638619423</v>
+        <v>0.1246255412697792</v>
       </c>
       <c r="G53">
-        <v>0.9988041520118713</v>
+        <v>0.8957404494285583</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2066,22 +2066,22 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.1499686390161514</v>
+        <v>-0.6995952725410461</v>
       </c>
       <c r="C54">
-        <v>0.0215346273034811</v>
+        <v>-0.9130571484565735</v>
       </c>
       <c r="D54">
         <v>-0.1165135279297829</v>
       </c>
       <c r="E54">
-        <v>-0.9887804985046387</v>
+        <v>-0.9964092373847961</v>
       </c>
       <c r="F54">
-        <v>0.03973514959216118</v>
+        <v>-0.08501014113426208</v>
       </c>
       <c r="G54">
-        <v>-0.9610294103622437</v>
+        <v>-0.9991627931594849</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2089,22 +2089,22 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.04187830910086632</v>
+        <v>-0.5933790802955627</v>
       </c>
       <c r="C55">
-        <v>-0.2173748165369034</v>
+        <v>-0.6183627843856812</v>
       </c>
       <c r="D55">
         <v>0.04982072860002518</v>
       </c>
       <c r="E55">
-        <v>-0.8546743988990784</v>
+        <v>-0.888873815536499</v>
       </c>
       <c r="F55">
-        <v>0.0003158923937007785</v>
+        <v>-0.05799109488725662</v>
       </c>
       <c r="G55">
-        <v>-0.9859594702720642</v>
+        <v>-0.8918868899345398</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2112,22 +2112,22 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>-0.07402279227972031</v>
+        <v>-0.09552368521690369</v>
       </c>
       <c r="C56">
-        <v>-0.3751841187477112</v>
+        <v>-0.5613293647766113</v>
       </c>
       <c r="D56">
         <v>2.553369631641544E-05</v>
       </c>
       <c r="E56">
-        <v>-0.4097961783409119</v>
+        <v>-0.8503060936927795</v>
       </c>
       <c r="F56">
-        <v>-0.01568553410470486</v>
+        <v>0.005709873046725988</v>
       </c>
       <c r="G56">
-        <v>-0.7295601367950439</v>
+        <v>-0.71161949634552</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2135,22 +2135,22 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.07218576967716217</v>
+        <v>-0.2726937830448151</v>
       </c>
       <c r="C57">
-        <v>-0.478457897901535</v>
+        <v>-0.5788652896881104</v>
       </c>
       <c r="D57">
         <v>0.04419801756739616</v>
       </c>
       <c r="E57">
-        <v>-0.9846866726875305</v>
+        <v>-0.9703985452651978</v>
       </c>
       <c r="F57">
-        <v>-0.0107232453301549</v>
+        <v>-0.04671872407197952</v>
       </c>
       <c r="G57">
-        <v>-0.9731175303459167</v>
+        <v>-0.9183475971221924</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2158,22 +2158,22 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>-0.2506773769855499</v>
+        <v>-0.0965261310338974</v>
       </c>
       <c r="C58">
-        <v>-0.5178741812705994</v>
+        <v>-0.8199467658996582</v>
       </c>
       <c r="D58">
         <v>0.00839912798255682</v>
       </c>
       <c r="E58">
-        <v>-0.9917400479316711</v>
+        <v>-0.8803818225860596</v>
       </c>
       <c r="F58">
-        <v>0.03001423552632332</v>
+        <v>-0.05421264842152596</v>
       </c>
       <c r="G58">
-        <v>-0.631092369556427</v>
+        <v>-0.6890895962715149</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2181,22 +2181,22 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>-0.03692600876092911</v>
+        <v>-0.2504352331161499</v>
       </c>
       <c r="C59">
-        <v>-0.2852423191070557</v>
+        <v>-0.6902534365653992</v>
       </c>
       <c r="D59">
         <v>0.08661159873008728</v>
       </c>
       <c r="E59">
-        <v>-0.9837088584899902</v>
+        <v>-0.5088853240013123</v>
       </c>
       <c r="F59">
-        <v>-0.006714893970638514</v>
+        <v>0.1286438256502151</v>
       </c>
       <c r="G59">
-        <v>-0.6171792149543762</v>
+        <v>-0.4043039679527283</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2204,22 +2204,22 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.006761695723980665</v>
+        <v>-0.7481542229652405</v>
       </c>
       <c r="C60">
-        <v>-0.7748593091964722</v>
+        <v>-0.9260876178741455</v>
       </c>
       <c r="D60">
         <v>0.04343678802251816</v>
       </c>
       <c r="E60">
-        <v>-0.9997515082359314</v>
+        <v>-0.8822267651557922</v>
       </c>
       <c r="F60">
-        <v>-0.04245597869157791</v>
+        <v>0.05958912521600723</v>
       </c>
       <c r="G60">
-        <v>-0.9908306002616882</v>
+        <v>-0.8888078331947327</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2227,22 +2227,22 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.03026850707828999</v>
+        <v>-0.05478078126907349</v>
       </c>
       <c r="C61">
-        <v>-0.5492133498191833</v>
+        <v>-0.1459669023752213</v>
       </c>
       <c r="D61">
         <v>0.02130724675953388</v>
       </c>
       <c r="E61">
-        <v>-0.9832075238227844</v>
+        <v>-0.9955419898033142</v>
       </c>
       <c r="F61">
-        <v>-0.01501049194484949</v>
+        <v>-0.04041710495948792</v>
       </c>
       <c r="G61">
-        <v>-0.919796884059906</v>
+        <v>-0.9867478013038635</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2250,22 +2250,22 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>-0.02452839910984039</v>
+        <v>-0.1383964866399765</v>
       </c>
       <c r="C62">
-        <v>-0.4916732013225555</v>
+        <v>-0.7764450311660767</v>
       </c>
       <c r="D62">
         <v>-0.02799495495855808</v>
       </c>
       <c r="E62">
-        <v>-0.9143021702766418</v>
+        <v>-0.998394250869751</v>
       </c>
       <c r="F62">
-        <v>0.01435667369514704</v>
+        <v>-0.07884988933801651</v>
       </c>
       <c r="G62">
-        <v>-0.9949610829353333</v>
+        <v>-0.9903623461723328</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2273,22 +2273,22 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>-0.06716191023588181</v>
+        <v>-0.5401403307914734</v>
       </c>
       <c r="C63">
-        <v>-0.5277255177497864</v>
+        <v>-0.9084506034851074</v>
       </c>
       <c r="D63">
         <v>-0.04002542793750763</v>
       </c>
       <c r="E63">
-        <v>-0.932665228843689</v>
+        <v>-0.8520251512527466</v>
       </c>
       <c r="F63">
-        <v>-0.02645652741193771</v>
+        <v>0.08543668687343597</v>
       </c>
       <c r="G63">
-        <v>-0.9993774890899658</v>
+        <v>-0.962422788143158</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2296,22 +2296,22 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>-0.005505301523953676</v>
+        <v>0.4102546274662018</v>
       </c>
       <c r="C64">
-        <v>-0.6271055340766907</v>
+        <v>-0.9445947408676147</v>
       </c>
       <c r="D64">
         <v>-0.07249505072832108</v>
       </c>
       <c r="E64">
-        <v>-0.9342530965805054</v>
+        <v>-0.9983340501785278</v>
       </c>
       <c r="F64">
-        <v>0.03190212324261665</v>
+        <v>-0.1189567744731903</v>
       </c>
       <c r="G64">
-        <v>-0.9846771955490112</v>
+        <v>-0.8717498779296875</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2319,22 +2319,22 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.1080440282821655</v>
+        <v>-0.1016935333609581</v>
       </c>
       <c r="C65">
-        <v>0.08763152360916138</v>
+        <v>-0.05782248824834824</v>
       </c>
       <c r="D65">
         <v>0.01539157796651125</v>
       </c>
       <c r="E65">
-        <v>-0.208327516913414</v>
+        <v>-0.7125522494316101</v>
       </c>
       <c r="F65">
-        <v>-0.02990189008414745</v>
+        <v>-0.02839631587266922</v>
       </c>
       <c r="G65">
-        <v>-0.638160228729248</v>
+        <v>-0.3691596984863281</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2342,22 +2342,22 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.1145292520523071</v>
+        <v>-0.3385889232158661</v>
       </c>
       <c r="C66">
-        <v>0.430409699678421</v>
+        <v>-0.4557766616344452</v>
       </c>
       <c r="D66">
         <v>0.1102180629968643</v>
       </c>
       <c r="E66">
-        <v>-0.3958702981472015</v>
+        <v>-0.01210917811840773</v>
       </c>
       <c r="F66">
-        <v>-0.03308865055441856</v>
+        <v>0.06453512609004974</v>
       </c>
       <c r="G66">
-        <v>0.0962008610367775</v>
+        <v>0.1197750121355057</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2365,22 +2365,22 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.01536709535866976</v>
+        <v>-0.2513171434402466</v>
       </c>
       <c r="C67">
-        <v>-0.2984265685081482</v>
+        <v>-0.8472210764884949</v>
       </c>
       <c r="D67">
         <v>-0.04133175313472748</v>
       </c>
       <c r="E67">
-        <v>-0.6170945763587952</v>
+        <v>-0.8363855481147766</v>
       </c>
       <c r="F67">
-        <v>-0.009550523944199085</v>
+        <v>-0.003178951796144247</v>
       </c>
       <c r="G67">
-        <v>-0.9436835050582886</v>
+        <v>-0.7087430357933044</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2388,22 +2388,22 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.09664678573608398</v>
+        <v>-0.5336882472038269</v>
       </c>
       <c r="C68">
-        <v>-0.1740891933441162</v>
+        <v>-0.9775222539901733</v>
       </c>
       <c r="D68">
         <v>0.001518504577688873</v>
       </c>
       <c r="E68">
-        <v>-0.908028781414032</v>
+        <v>0.8389898538589478</v>
       </c>
       <c r="F68">
-        <v>-0.06388114392757416</v>
+        <v>0.07457707822322845</v>
       </c>
       <c r="G68">
-        <v>-0.9947534203529358</v>
+        <v>0.7424574494361877</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2411,22 +2411,22 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>-0.0958152711391449</v>
+        <v>-0.673175573348999</v>
       </c>
       <c r="C69">
-        <v>-0.4598581790924072</v>
+        <v>-0.7370129227638245</v>
       </c>
       <c r="D69">
         <v>-0.08485125005245209</v>
       </c>
       <c r="E69">
-        <v>-0.4437925815582275</v>
+        <v>-0.8136448264122009</v>
       </c>
       <c r="F69">
-        <v>0.05432090163230896</v>
+        <v>-0.008128425106406212</v>
       </c>
       <c r="G69">
-        <v>0.494608610868454</v>
+        <v>-0.8814769387245178</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2434,22 +2434,22 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.04710284993052483</v>
+        <v>-0.7781918048858643</v>
       </c>
       <c r="C70">
-        <v>-0.8920984268188477</v>
+        <v>-0.9455749988555908</v>
       </c>
       <c r="D70">
         <v>0.1326808035373688</v>
       </c>
       <c r="E70">
-        <v>-0.9993841648101807</v>
+        <v>-0.9734221696853638</v>
       </c>
       <c r="F70">
-        <v>-0.03255967795848846</v>
+        <v>0.03536940738558769</v>
       </c>
       <c r="G70">
-        <v>-0.3659063279628754</v>
+        <v>-0.9951236844062805</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2457,22 +2457,22 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.004737394861876965</v>
+        <v>0.1359349638223648</v>
       </c>
       <c r="C71">
-        <v>0.327846348285675</v>
+        <v>-0.09801851958036423</v>
       </c>
       <c r="D71">
         <v>0.07357670366764069</v>
       </c>
       <c r="E71">
-        <v>-0.8839613199234009</v>
+        <v>0.1965295225381851</v>
       </c>
       <c r="F71">
-        <v>0.02757032215595245</v>
+        <v>-0.07536900788545609</v>
       </c>
       <c r="G71">
-        <v>-0.931249737739563</v>
+        <v>-0.3861600756645203</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2480,22 +2480,22 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>-0.07577578723430634</v>
+        <v>-0.514218270778656</v>
       </c>
       <c r="C72">
-        <v>-0.5237939953804016</v>
+        <v>-0.7139593362808228</v>
       </c>
       <c r="D72">
         <v>-0.01415385399013758</v>
       </c>
       <c r="E72">
-        <v>-0.9030695557594299</v>
+        <v>-0.9921562075614929</v>
       </c>
       <c r="F72">
-        <v>-0.05012579262256622</v>
+        <v>-0.1796820163726807</v>
       </c>
       <c r="G72">
-        <v>-0.8403432369232178</v>
+        <v>-0.9783143997192383</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2503,22 +2503,22 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.1120150461792946</v>
+        <v>-0.4222524762153625</v>
       </c>
       <c r="C73">
-        <v>0.06476109474897385</v>
+        <v>-0.9093301296234131</v>
       </c>
       <c r="D73">
         <v>0.03187740594148636</v>
       </c>
       <c r="E73">
-        <v>-0.8162475824356079</v>
+        <v>-0.9991301894187927</v>
       </c>
       <c r="F73">
-        <v>0.04427879303693771</v>
+        <v>-0.1581583023071289</v>
       </c>
       <c r="G73">
-        <v>-0.946776807308197</v>
+        <v>-0.9984010457992554</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2526,22 +2526,22 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0.08104351907968521</v>
+        <v>-0.7576920390129089</v>
       </c>
       <c r="C74">
-        <v>-0.4727421402931213</v>
+        <v>-0.6671722531318665</v>
       </c>
       <c r="D74">
         <v>-0.06500987708568573</v>
       </c>
       <c r="E74">
-        <v>-0.8445902466773987</v>
+        <v>-0.7351689338684082</v>
       </c>
       <c r="F74">
-        <v>-0.02897915057837963</v>
+        <v>0.1296186894178391</v>
       </c>
       <c r="G74">
-        <v>-0.8770539164543152</v>
+        <v>-0.8711334466934204</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2549,22 +2549,22 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>-0.2766310274600983</v>
+        <v>-0.1047451570630074</v>
       </c>
       <c r="C75">
-        <v>-0.3619697391986847</v>
+        <v>0.01112795155495405</v>
       </c>
       <c r="D75">
         <v>0.05884972214698792</v>
       </c>
       <c r="E75">
-        <v>-0.9038732647895813</v>
+        <v>-0.5969239473342896</v>
       </c>
       <c r="F75">
-        <v>-0.03582222387194633</v>
+        <v>0.1184800714254379</v>
       </c>
       <c r="G75">
-        <v>-0.5727325081825256</v>
+        <v>-0.3769456744194031</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2572,22 +2572,22 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>-0.03288991376757622</v>
+        <v>-0.4114656448364258</v>
       </c>
       <c r="C76">
-        <v>-0.2343801110982895</v>
+        <v>-0.5087600946426392</v>
       </c>
       <c r="D76">
         <v>-0.00621551601216197</v>
       </c>
       <c r="E76">
-        <v>-0.4897260367870331</v>
+        <v>-0.734944224357605</v>
       </c>
       <c r="F76">
-        <v>0.01366207841783762</v>
+        <v>-0.0799729973077774</v>
       </c>
       <c r="G76">
-        <v>-0.7567910552024841</v>
+        <v>-0.8726913928985596</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2595,22 +2595,22 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>-0.004533672705292702</v>
+        <v>-0.3923004269599915</v>
       </c>
       <c r="C77">
-        <v>-0.3954689204692841</v>
+        <v>-0.9195812940597534</v>
       </c>
       <c r="D77">
         <v>-0.0660284161567688</v>
       </c>
       <c r="E77">
-        <v>-0.9805692434310913</v>
+        <v>-0.9974920749664307</v>
       </c>
       <c r="F77">
-        <v>0.01933471858501434</v>
+        <v>0.06754074245691299</v>
       </c>
       <c r="G77">
-        <v>-0.9033851027488708</v>
+        <v>-0.9956860542297363</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2618,22 +2618,22 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.01777697168290615</v>
+        <v>0.4276097416877747</v>
       </c>
       <c r="C78">
-        <v>0.0479835532605648</v>
+        <v>-0.599614679813385</v>
       </c>
       <c r="D78">
         <v>-0.03458810970187187</v>
       </c>
       <c r="E78">
-        <v>-0.9987838268280029</v>
+        <v>-0.9879062175750732</v>
       </c>
       <c r="F78">
-        <v>-0.01157333329319954</v>
+        <v>0.05618706345558167</v>
       </c>
       <c r="G78">
-        <v>-0.9990960955619812</v>
+        <v>-0.9902850389480591</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2641,22 +2641,22 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.06361639499664307</v>
+        <v>-0.7890955805778503</v>
       </c>
       <c r="C79">
-        <v>-0.5010408759117126</v>
+        <v>-0.9816840291023254</v>
       </c>
       <c r="D79">
         <v>-0.07440705597400665</v>
       </c>
       <c r="E79">
-        <v>-0.9650967121124268</v>
+        <v>-0.9971112012863159</v>
       </c>
       <c r="F79">
-        <v>0.03763331472873688</v>
+        <v>-0.07488831132650375</v>
       </c>
       <c r="G79">
-        <v>-0.9812104105949402</v>
+        <v>-0.9931948184967041</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2664,22 +2664,22 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.006939360871911049</v>
+        <v>-0.5259737968444824</v>
       </c>
       <c r="C80">
-        <v>-0.5171846747398376</v>
+        <v>-0.9160054922103882</v>
       </c>
       <c r="D80">
         <v>-0.1820351332426071</v>
       </c>
       <c r="E80">
-        <v>-0.9076079130172729</v>
+        <v>-0.8912500143051147</v>
       </c>
       <c r="F80">
-        <v>-0.0197528712451458</v>
+        <v>-0.04209145531058311</v>
       </c>
       <c r="G80">
-        <v>-0.9713301658630371</v>
+        <v>-0.9476616382598877</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2687,22 +2687,22 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>-0.04501552879810333</v>
+        <v>-0.6127995252609253</v>
       </c>
       <c r="C81">
-        <v>-0.1902604550123215</v>
+        <v>-0.8365902304649353</v>
       </c>
       <c r="D81">
         <v>0.0185608696192503</v>
       </c>
       <c r="E81">
-        <v>-0.2902688086032867</v>
+        <v>-0.9598098397254944</v>
       </c>
       <c r="F81">
-        <v>-0.02058922313153744</v>
+        <v>0.04623763635754585</v>
       </c>
       <c r="G81">
-        <v>-0.9591427445411682</v>
+        <v>-0.9558615684509277</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2710,22 +2710,22 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0.05435153096914291</v>
+        <v>0.1094977632164955</v>
       </c>
       <c r="C82">
-        <v>-0.00551350973546505</v>
+        <v>-0.925555408000946</v>
       </c>
       <c r="D82">
         <v>-0.05514155700802803</v>
       </c>
       <c r="E82">
-        <v>-0.7919774651527405</v>
+        <v>-0.8917428255081177</v>
       </c>
       <c r="F82">
-        <v>-0.04173144698143005</v>
+        <v>-0.09331152588129044</v>
       </c>
       <c r="G82">
-        <v>-0.9609615206718445</v>
+        <v>-0.9052091240882874</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2733,22 +2733,22 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0.02457967028021812</v>
+        <v>-0.3363509178161621</v>
       </c>
       <c r="C83">
-        <v>-0.3168641924858093</v>
+        <v>-0.9506169557571411</v>
       </c>
       <c r="D83">
         <v>0.05199674889445305</v>
       </c>
       <c r="E83">
-        <v>-0.9790750741958618</v>
+        <v>-0.9933822154998779</v>
       </c>
       <c r="F83">
-        <v>0.01269752345979214</v>
+        <v>0.04519856348633766</v>
       </c>
       <c r="G83">
-        <v>-0.9976196885108948</v>
+        <v>-0.9884863495826721</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2756,22 +2756,22 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>-0.1838096678256989</v>
+        <v>-0.3560776710510254</v>
       </c>
       <c r="C84">
-        <v>-0.7687466144561768</v>
+        <v>-0.8616920709609985</v>
       </c>
       <c r="D84">
         <v>-0.001561302226036787</v>
       </c>
       <c r="E84">
-        <v>-0.9496077299118042</v>
+        <v>-0.8954409956932068</v>
       </c>
       <c r="F84">
-        <v>0.01043099164962769</v>
+        <v>-0.06761091202497482</v>
       </c>
       <c r="G84">
-        <v>-0.5423303842544556</v>
+        <v>-0.917330801486969</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2779,22 +2779,22 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>-0.004347474314272404</v>
+        <v>-0.6190733909606934</v>
       </c>
       <c r="C85">
-        <v>-0.1754712611436844</v>
+        <v>-0.6688899993896484</v>
       </c>
       <c r="D85">
         <v>0.03934527933597565</v>
       </c>
       <c r="E85">
-        <v>-0.958142101764679</v>
+        <v>-0.9494799375534058</v>
       </c>
       <c r="F85">
-        <v>0.02344213798642159</v>
+        <v>-0.0916457399725914</v>
       </c>
       <c r="G85">
-        <v>-0.6102414131164551</v>
+        <v>-0.7275314927101135</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2802,22 +2802,22 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0.2242589443922043</v>
+        <v>-0.05858425796031952</v>
       </c>
       <c r="C86">
-        <v>-0.8129259347915649</v>
+        <v>-0.9675452709197998</v>
       </c>
       <c r="D86">
         <v>-0.08306356519460678</v>
       </c>
       <c r="E86">
-        <v>-0.9225435256958008</v>
+        <v>-0.6227695345878601</v>
       </c>
       <c r="F86">
-        <v>0.03542521595954895</v>
+        <v>0.05537916347384453</v>
       </c>
       <c r="G86">
-        <v>-0.8868690729141235</v>
+        <v>0.2576198279857635</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2825,22 +2825,22 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>-0.01541339419782162</v>
+        <v>-0.03725852444767952</v>
       </c>
       <c r="C87">
-        <v>-0.5040361285209656</v>
+        <v>-0.798255980014801</v>
       </c>
       <c r="D87">
         <v>0.01306915562599897</v>
       </c>
       <c r="E87">
-        <v>-0.9965340495109558</v>
+        <v>-0.3608973324298859</v>
       </c>
       <c r="F87">
-        <v>-0.05877625569701195</v>
+        <v>0.1299096047878265</v>
       </c>
       <c r="G87">
-        <v>-0.9915931224822998</v>
+        <v>-0.7675504684448242</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2848,22 +2848,22 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>-0.02598397806286812</v>
+        <v>-0.4754632711410522</v>
       </c>
       <c r="C88">
-        <v>-0.3565341532230377</v>
+        <v>-0.7619979977607727</v>
       </c>
       <c r="D88">
         <v>-0.01770670898258686</v>
       </c>
       <c r="E88">
-        <v>-0.7974194884300232</v>
+        <v>-0.9913010597229004</v>
       </c>
       <c r="F88">
-        <v>0.003739481559023261</v>
+        <v>-0.07533377408981323</v>
       </c>
       <c r="G88">
-        <v>-0.9613581299781799</v>
+        <v>-0.9438381791114807</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2871,22 +2871,22 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>-0.01303684897720814</v>
+        <v>-0.4086735546588898</v>
       </c>
       <c r="C89">
-        <v>-0.6206470131874084</v>
+        <v>-0.6793587803840637</v>
       </c>
       <c r="D89">
         <v>-0.0718986913561821</v>
       </c>
       <c r="E89">
-        <v>-0.9536926746368408</v>
+        <v>-0.9710748195648193</v>
       </c>
       <c r="F89">
-        <v>0.008933163248002529</v>
+        <v>-0.1519690304994583</v>
       </c>
       <c r="G89">
-        <v>-0.9467751979827881</v>
+        <v>-0.8444426655769348</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2894,22 +2894,22 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.1829978376626968</v>
+        <v>-0.7714307904243469</v>
       </c>
       <c r="C90">
-        <v>-0.6819595694541931</v>
+        <v>-0.8850536346435547</v>
       </c>
       <c r="D90">
         <v>0.03027123212814331</v>
       </c>
       <c r="E90">
-        <v>-0.9661563634872437</v>
+        <v>-0.9907168745994568</v>
       </c>
       <c r="F90">
-        <v>-0.01110104471445084</v>
+        <v>0.06772292405366898</v>
       </c>
       <c r="G90">
-        <v>-0.9721959233283997</v>
+        <v>-0.9822797179222107</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2917,22 +2917,22 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>-0.0913139283657074</v>
+        <v>-0.570788562297821</v>
       </c>
       <c r="C91">
-        <v>0.135891392827034</v>
+        <v>-0.9394374489784241</v>
       </c>
       <c r="D91">
         <v>0.03444895148277283</v>
       </c>
       <c r="E91">
-        <v>0.2733848392963409</v>
+        <v>-0.131428137421608</v>
       </c>
       <c r="F91">
-        <v>0.008644257672131062</v>
+        <v>0.0479879155755043</v>
       </c>
       <c r="G91">
-        <v>-0.9594628810882568</v>
+        <v>-0.0386299267411232</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2940,22 +2940,22 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>-0.02611230127513409</v>
+        <v>-0.8810173869132996</v>
       </c>
       <c r="C92">
-        <v>-0.7966541051864624</v>
+        <v>-0.9639235138893127</v>
       </c>
       <c r="D92">
         <v>-0.02065654844045639</v>
       </c>
       <c r="E92">
-        <v>-0.9986861944198608</v>
+        <v>-0.9978920817375183</v>
       </c>
       <c r="F92">
-        <v>-0.007020207121968269</v>
+        <v>-0.1306749135255814</v>
       </c>
       <c r="G92">
-        <v>-0.1592008173465729</v>
+        <v>-0.972714900970459</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2963,22 +2963,22 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.05972273275256157</v>
+        <v>-0.5699328780174255</v>
       </c>
       <c r="C93">
-        <v>-0.1622631996870041</v>
+        <v>-0.8659435510635376</v>
       </c>
       <c r="D93">
         <v>0.01499569974839687</v>
       </c>
       <c r="E93">
-        <v>-0.08519568294286728</v>
+        <v>-0.9709103107452393</v>
       </c>
       <c r="F93">
-        <v>0.0386868342757225</v>
+        <v>-0.06166421249508858</v>
       </c>
       <c r="G93">
-        <v>-0.9012172818183899</v>
+        <v>-0.8487690091133118</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2986,22 +2986,22 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.09489756077528</v>
+        <v>-0.8144698739051819</v>
       </c>
       <c r="C94">
-        <v>-0.4994827806949615</v>
+        <v>-0.990675687789917</v>
       </c>
       <c r="D94">
         <v>-0.005723177455365658</v>
       </c>
       <c r="E94">
-        <v>-0.9985817670822144</v>
+        <v>-0.8136671781539917</v>
       </c>
       <c r="F94">
-        <v>-0.02560451254248619</v>
+        <v>0.02618470415472984</v>
       </c>
       <c r="G94">
-        <v>-0.5470969676971436</v>
+        <v>-0.9812203049659729</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -3009,22 +3009,22 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>-0.1107451170682907</v>
+        <v>0.3751207888126373</v>
       </c>
       <c r="C95">
-        <v>-0.4687530100345612</v>
+        <v>0.2798797190189362</v>
       </c>
       <c r="D95">
         <v>-0.05011462792754173</v>
       </c>
       <c r="E95">
-        <v>-0.2977405190467834</v>
+        <v>-0.3104681968688965</v>
       </c>
       <c r="F95">
-        <v>-0.04538558050990105</v>
+        <v>-0.05666635930538177</v>
       </c>
       <c r="G95">
-        <v>-0.8596195578575134</v>
+        <v>-0.3773891925811768</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -3032,22 +3032,22 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>-0.2672575712203979</v>
+        <v>-0.7097067832946777</v>
       </c>
       <c r="C96">
-        <v>-0.8538599014282227</v>
+        <v>-0.8456354141235352</v>
       </c>
       <c r="D96">
         <v>0.05684319138526917</v>
       </c>
       <c r="E96">
-        <v>-0.9677174091339111</v>
+        <v>-0.9998509883880615</v>
       </c>
       <c r="F96">
-        <v>-0.03203139081597328</v>
+        <v>-0.1043156981468201</v>
       </c>
       <c r="G96">
-        <v>-0.9911664128303528</v>
+        <v>-0.9920555353164673</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -3055,22 +3055,22 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>-0.02686583623290062</v>
+        <v>-0.09823755174875259</v>
       </c>
       <c r="C97">
-        <v>-0.1061945632100105</v>
+        <v>-0.9160642027854919</v>
       </c>
       <c r="D97">
         <v>-0.04477493464946747</v>
       </c>
       <c r="E97">
-        <v>0.06793089210987091</v>
+        <v>-0.921609103679657</v>
       </c>
       <c r="F97">
-        <v>0.0002687984961085021</v>
+        <v>0.1124914884567261</v>
       </c>
       <c r="G97">
-        <v>-0.7694990634918213</v>
+        <v>-0.5270951390266418</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -3078,22 +3078,22 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>0.12909235060215</v>
+        <v>-0.3787154853343964</v>
       </c>
       <c r="C98">
-        <v>-0.3355697393417358</v>
+        <v>-0.8694542050361633</v>
       </c>
       <c r="D98">
         <v>0.004700540099292994</v>
       </c>
       <c r="E98">
-        <v>-0.9888787269592285</v>
+        <v>-0.9327529668807983</v>
       </c>
       <c r="F98">
-        <v>0.02272355929017067</v>
+        <v>-0.1014250814914703</v>
       </c>
       <c r="G98">
-        <v>-0.4945206344127655</v>
+        <v>-0.2204903662204742</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -3101,22 +3101,22 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>-0.1860174387693405</v>
+        <v>-0.5038995742797852</v>
       </c>
       <c r="C99">
-        <v>-0.3151289224624634</v>
+        <v>-0.682390034198761</v>
       </c>
       <c r="D99">
         <v>0.008064404129981995</v>
       </c>
       <c r="E99">
-        <v>-0.5512829422950745</v>
+        <v>-0.8877558708190918</v>
       </c>
       <c r="F99">
-        <v>-0.04749412089586258</v>
+        <v>0.007993406616151333</v>
       </c>
       <c r="G99">
-        <v>-0.8235171437263489</v>
+        <v>-0.8737137317657471</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -3124,22 +3124,22 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>-0.03249039873480797</v>
+        <v>-0.1278498321771622</v>
       </c>
       <c r="C100">
-        <v>0.1555229276418686</v>
+        <v>-0.808177649974823</v>
       </c>
       <c r="D100">
         <v>0.04984112456440926</v>
       </c>
       <c r="E100">
-        <v>0.4023484289646149</v>
+        <v>0.4457261264324188</v>
       </c>
       <c r="F100">
-        <v>-0.01217754650861025</v>
+        <v>-0.03230298310518265</v>
       </c>
       <c r="G100">
-        <v>-0.9220106601715088</v>
+        <v>0.7423064708709717</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -3147,22 +3147,22 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0.1405115276575089</v>
+        <v>-0.9493387341499329</v>
       </c>
       <c r="C101">
-        <v>-0.6946335434913635</v>
+        <v>-0.9949596524238586</v>
       </c>
       <c r="D101">
         <v>-0.07787472754716873</v>
       </c>
       <c r="E101">
-        <v>-0.983863353729248</v>
+        <v>-0.9994944334030151</v>
       </c>
       <c r="F101">
-        <v>0.02691071294248104</v>
+        <v>0.006558051332831383</v>
       </c>
       <c r="G101">
-        <v>-0.9933938384056091</v>
+        <v>-0.9952071309089661</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -3170,22 +3170,22 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>-0.0681922659277916</v>
+        <v>-0.4207226037979126</v>
       </c>
       <c r="C102">
-        <v>0.04262842610478401</v>
+        <v>-0.9263609051704407</v>
       </c>
       <c r="D102">
         <v>-0.04626800864934921</v>
       </c>
       <c r="E102">
-        <v>-0.5532649159431458</v>
+        <v>-0.6699308156967163</v>
       </c>
       <c r="F102">
-        <v>0.00267178425565362</v>
+        <v>0.1177296787500381</v>
       </c>
       <c r="G102">
-        <v>-0.9119971394538879</v>
+        <v>-0.2459527403116226</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -3193,22 +3193,22 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>-0.07039130479097366</v>
+        <v>-0.4282366037368774</v>
       </c>
       <c r="C103">
-        <v>-0.3046775758266449</v>
+        <v>-0.8988634943962097</v>
       </c>
       <c r="D103">
         <v>0.02838541194796562</v>
       </c>
       <c r="E103">
-        <v>-0.7891296744346619</v>
+        <v>0.8365031480789185</v>
       </c>
       <c r="F103">
-        <v>-0.04326845705509186</v>
+        <v>0.09869235754013062</v>
       </c>
       <c r="G103">
-        <v>-0.9563394784927368</v>
+        <v>0.7304008603096008</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -3216,22 +3216,22 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>-0.2270461022853851</v>
+        <v>0.4353663623332977</v>
       </c>
       <c r="C104">
-        <v>-0.8767887949943542</v>
+        <v>-0.4902960062026978</v>
       </c>
       <c r="D104">
         <v>0.05039457231760025</v>
       </c>
       <c r="E104">
-        <v>-0.9566403031349182</v>
+        <v>-0.8344710469245911</v>
       </c>
       <c r="F104">
-        <v>0.07721824198961258</v>
+        <v>-0.1719720810651779</v>
       </c>
       <c r="G104">
-        <v>-0.9173120856285095</v>
+        <v>-0.465422660112381</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -3239,22 +3239,22 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>0.09105987101793289</v>
+        <v>-0.6652794480323792</v>
       </c>
       <c r="C105">
-        <v>-0.7032415866851807</v>
+        <v>-0.9722719788551331</v>
       </c>
       <c r="D105">
         <v>-0.1058031991124153</v>
       </c>
       <c r="E105">
-        <v>-0.9883401393890381</v>
+        <v>-0.7975628972053528</v>
       </c>
       <c r="F105">
-        <v>0.01360167842358351</v>
+        <v>-0.02614385075867176</v>
       </c>
       <c r="G105">
-        <v>-0.9854832291603088</v>
+        <v>-0.7610522508621216</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -3262,22 +3262,22 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>-0.2280630171298981</v>
+        <v>-0.3793547749519348</v>
       </c>
       <c r="C106">
-        <v>-0.7809756398200989</v>
+        <v>-0.4339036643505096</v>
       </c>
       <c r="D106">
         <v>0.0008670181850902736</v>
       </c>
       <c r="E106">
-        <v>-0.9992328286170959</v>
+        <v>-0.8683522343635559</v>
       </c>
       <c r="F106">
-        <v>-0.001186156761832535</v>
+        <v>0.04497367888689041</v>
       </c>
       <c r="G106">
-        <v>-0.8311095237731934</v>
+        <v>-0.5584746599197388</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -3285,22 +3285,22 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>-0.04519488662481308</v>
+        <v>0.1495617628097534</v>
       </c>
       <c r="C107">
-        <v>0.1687581092119217</v>
+        <v>-0.8983210325241089</v>
       </c>
       <c r="D107">
         <v>0.02810205519199371</v>
       </c>
       <c r="E107">
-        <v>-0.8672946095466614</v>
+        <v>-0.9966323971748352</v>
       </c>
       <c r="F107">
-        <v>0.002010267926380038</v>
+        <v>-0.0124118234962225</v>
       </c>
       <c r="G107">
-        <v>0.2970139980316162</v>
+        <v>-0.9760618209838867</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -3308,22 +3308,22 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>-0.02045634016394615</v>
+        <v>-0.5494213700294495</v>
       </c>
       <c r="C108">
-        <v>-0.3630903959274292</v>
+        <v>-0.7586065530776978</v>
       </c>
       <c r="D108">
         <v>-0.02512850239872932</v>
       </c>
       <c r="E108">
-        <v>-0.9803276658058167</v>
+        <v>-0.9918155670166016</v>
       </c>
       <c r="F108">
-        <v>0.01453555747866631</v>
+        <v>-0.0713399350643158</v>
       </c>
       <c r="G108">
-        <v>-0.696147620677948</v>
+        <v>-0.9874719381332397</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -3331,22 +3331,22 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>-0.04743413999676704</v>
+        <v>0.3967428207397461</v>
       </c>
       <c r="C109">
-        <v>-0.1710705608129501</v>
+        <v>-0.5179100036621094</v>
       </c>
       <c r="D109">
         <v>-0.04419492185115814</v>
       </c>
       <c r="E109">
-        <v>-0.59866863489151</v>
+        <v>-0.8463367819786072</v>
       </c>
       <c r="F109">
-        <v>-0.002360814949497581</v>
+        <v>0.1112123653292656</v>
       </c>
       <c r="G109">
-        <v>-0.815483570098877</v>
+        <v>-0.9416458606719971</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -3354,22 +3354,22 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>-0.2299737185239792</v>
+        <v>-0.7186733484268188</v>
       </c>
       <c r="C110">
-        <v>-0.550504744052887</v>
+        <v>-0.9315034747123718</v>
       </c>
       <c r="D110">
         <v>-0.03037906251847744</v>
       </c>
       <c r="E110">
-        <v>-0.9997724890708923</v>
+        <v>-0.9012721180915833</v>
       </c>
       <c r="F110">
-        <v>-0.04093221947550774</v>
+        <v>-0.06705302000045776</v>
       </c>
       <c r="G110">
-        <v>-0.98456871509552</v>
+        <v>-0.9860345125198364</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -3377,22 +3377,22 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>-0.1414933055639267</v>
+        <v>-0.3977074921131134</v>
       </c>
       <c r="C111">
-        <v>-0.6946538090705872</v>
+        <v>-0.5918236970901489</v>
       </c>
       <c r="D111">
         <v>0.03581491485238075</v>
       </c>
       <c r="E111">
-        <v>-0.9761203527450562</v>
+        <v>0.6143827438354492</v>
       </c>
       <c r="F111">
-        <v>-0.03218284249305725</v>
+        <v>0.03747325390577316</v>
       </c>
       <c r="G111">
-        <v>0.09048625826835632</v>
+        <v>0.4979087114334106</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -3400,22 +3400,22 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>-0.06724794954061508</v>
+        <v>-0.6746889352798462</v>
       </c>
       <c r="C112">
-        <v>0.04491440206766129</v>
+        <v>-0.4969743192195892</v>
       </c>
       <c r="D112">
         <v>0.120218500494957</v>
       </c>
       <c r="E112">
-        <v>-0.8365457057952881</v>
+        <v>-0.7974792718887329</v>
       </c>
       <c r="F112">
-        <v>-0.04792346432805061</v>
+        <v>-0.0839383453130722</v>
       </c>
       <c r="G112">
-        <v>-0.9893691539764404</v>
+        <v>-0.9651246070861816</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -3423,22 +3423,22 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>-0.05095575749874115</v>
+        <v>-0.2979661524295807</v>
       </c>
       <c r="C113">
-        <v>-0.1050588339567184</v>
+        <v>-0.743743896484375</v>
       </c>
       <c r="D113">
         <v>-0.02110435999929905</v>
       </c>
       <c r="E113">
-        <v>-0.8949040770530701</v>
+        <v>-0.6454253792762756</v>
       </c>
       <c r="F113">
-        <v>-0.003775476012378931</v>
+        <v>-0.07840486615896225</v>
       </c>
       <c r="G113">
-        <v>-0.9390031099319458</v>
+        <v>-0.7739788889884949</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3446,22 +3446,22 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>0.1019302532076836</v>
+        <v>0.07299020886421204</v>
       </c>
       <c r="C114">
-        <v>0.1443810015916824</v>
+        <v>-0.02463746070861816</v>
       </c>
       <c r="D114">
         <v>0.08630994707345963</v>
       </c>
       <c r="E114">
-        <v>-0.9103642702102661</v>
+        <v>-0.9496728777885437</v>
       </c>
       <c r="F114">
-        <v>-0.0678069069981575</v>
+        <v>0.004803646355867386</v>
       </c>
       <c r="G114">
-        <v>-0.9025678038597107</v>
+        <v>-0.7090194225311279</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3469,22 +3469,22 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>-0.1988438814878464</v>
+        <v>-0.6776719093322754</v>
       </c>
       <c r="C115">
-        <v>-0.1449826210737228</v>
+        <v>-0.7207064032554626</v>
       </c>
       <c r="D115">
         <v>0.03171446174383163</v>
       </c>
       <c r="E115">
-        <v>-0.7385850548744202</v>
+        <v>-0.8535826802253723</v>
       </c>
       <c r="F115">
-        <v>-0.0087841572239995</v>
+        <v>0.09989863634109497</v>
       </c>
       <c r="G115">
-        <v>-0.8604671955108643</v>
+        <v>-0.698448657989502</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3492,22 +3492,22 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>-0.005339129827916622</v>
+        <v>-0.5016843676567078</v>
       </c>
       <c r="C116">
-        <v>-0.1656158268451691</v>
+        <v>-0.6944592595100403</v>
       </c>
       <c r="D116">
         <v>0.1080950647592545</v>
       </c>
       <c r="E116">
-        <v>-0.9956865310668945</v>
+        <v>-0.9730661511421204</v>
       </c>
       <c r="F116">
-        <v>-0.00330216926522553</v>
+        <v>0.04075875505805016</v>
       </c>
       <c r="G116">
-        <v>0.1778162568807602</v>
+        <v>-0.9730172157287598</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3515,22 +3515,22 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>-0.07073206454515457</v>
+        <v>-0.5210763812065125</v>
       </c>
       <c r="C117">
-        <v>-0.2851845026016235</v>
+        <v>-0.8814920783042908</v>
       </c>
       <c r="D117">
         <v>-0.02042775973677635</v>
       </c>
       <c r="E117">
-        <v>-0.7278726100921631</v>
+        <v>-0.8314615488052368</v>
       </c>
       <c r="F117">
-        <v>0.004789546597748995</v>
+        <v>-0.05602145940065384</v>
       </c>
       <c r="G117">
-        <v>-0.8089954257011414</v>
+        <v>-0.6911029815673828</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3538,22 +3538,22 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>0.3046062588691711</v>
+        <v>0.7613315582275391</v>
       </c>
       <c r="C118">
-        <v>-0.5807047486305237</v>
+        <v>-0.9202122092247009</v>
       </c>
       <c r="D118">
         <v>-0.1270650178194046</v>
       </c>
       <c r="E118">
-        <v>-0.9750684499740601</v>
+        <v>-0.9985759258270264</v>
       </c>
       <c r="F118">
-        <v>-0.00309009850025177</v>
+        <v>0.02937600016593933</v>
       </c>
       <c r="G118">
-        <v>-0.6752552390098572</v>
+        <v>-0.9483929872512817</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3561,22 +3561,22 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>0.1396129876375198</v>
+        <v>-0.6088537573814392</v>
       </c>
       <c r="C119">
-        <v>-0.06531179696321487</v>
+        <v>-0.74651700258255</v>
       </c>
       <c r="D119">
         <v>0.008727528154850006</v>
       </c>
       <c r="E119">
-        <v>-0.9306275844573975</v>
+        <v>-0.2782704830169678</v>
       </c>
       <c r="F119">
-        <v>-0.002103510312736034</v>
+        <v>0.01639789156615734</v>
       </c>
       <c r="G119">
-        <v>-0.5743732452392578</v>
+        <v>-0.4776932597160339</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3584,22 +3584,22 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>0.19643834233284</v>
+        <v>-0.8265860676765442</v>
       </c>
       <c r="C120">
-        <v>-0.643288254737854</v>
+        <v>-0.9812141060829163</v>
       </c>
       <c r="D120">
         <v>0.01849262975156307</v>
       </c>
       <c r="E120">
-        <v>-0.7141093015670776</v>
+        <v>-0.9874141216278076</v>
       </c>
       <c r="F120">
-        <v>-0.02984862960875034</v>
+        <v>0.1135107427835464</v>
       </c>
       <c r="G120">
-        <v>-0.6983901262283325</v>
+        <v>-0.925628125667572</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3607,22 +3607,22 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>-0.2543146312236786</v>
+        <v>0.04972098395228386</v>
       </c>
       <c r="C121">
-        <v>-0.5263651609420776</v>
+        <v>-0.8077342510223389</v>
       </c>
       <c r="D121">
         <v>-0.05713560804724693</v>
       </c>
       <c r="E121">
-        <v>-0.7159101366996765</v>
+        <v>-0.2674500942230225</v>
       </c>
       <c r="F121">
-        <v>0.03880545869469643</v>
+        <v>-0.01364369224756956</v>
       </c>
       <c r="G121">
-        <v>-0.6121460795402527</v>
+        <v>-0.0601896196603775</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3630,22 +3630,22 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>-0.08631099760532379</v>
+        <v>-0.5656896829605103</v>
       </c>
       <c r="C122">
-        <v>-0.6844949126243591</v>
+        <v>-0.9765872955322266</v>
       </c>
       <c r="D122">
         <v>-0.1252989172935486</v>
       </c>
       <c r="E122">
-        <v>-0.8185204863548279</v>
+        <v>-0.8581695556640625</v>
       </c>
       <c r="F122">
-        <v>0.002724551362916827</v>
+        <v>-0.06789843738079071</v>
       </c>
       <c r="G122">
-        <v>-0.8541221618652344</v>
+        <v>-0.6412753462791443</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3653,22 +3653,22 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>-0.07928476482629776</v>
+        <v>-0.4088946580886841</v>
       </c>
       <c r="C123">
-        <v>-0.9004484415054321</v>
+        <v>-0.642052948474884</v>
       </c>
       <c r="D123">
         <v>-0.05216264724731445</v>
       </c>
       <c r="E123">
-        <v>-0.9843527674674988</v>
+        <v>-0.6893370151519775</v>
       </c>
       <c r="F123">
-        <v>0.02761762775480747</v>
+        <v>0.03808300569653511</v>
       </c>
       <c r="G123">
-        <v>-0.9513072371482849</v>
+        <v>0.4509739875793457</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3676,22 +3676,22 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>-0.0379612073302269</v>
+        <v>-0.2611192166805267</v>
       </c>
       <c r="C124">
-        <v>0.2997175455093384</v>
+        <v>0.3623327612876892</v>
       </c>
       <c r="D124">
         <v>0.05561525002121925</v>
       </c>
       <c r="E124">
-        <v>-0.9865128397941589</v>
+        <v>-0.9963347315788269</v>
       </c>
       <c r="F124">
-        <v>0.04161863029003143</v>
+        <v>-0.02840550616383553</v>
       </c>
       <c r="G124">
-        <v>-0.7147427201271057</v>
+        <v>-0.7918075919151306</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3699,22 +3699,22 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>-0.2414992302656174</v>
+        <v>-0.4062864184379578</v>
       </c>
       <c r="C125">
-        <v>-0.4303675889968872</v>
+        <v>-0.7414246201515198</v>
       </c>
       <c r="D125">
         <v>0.02631143666803837</v>
       </c>
       <c r="E125">
-        <v>-0.6606870293617249</v>
+        <v>0.9265121221542358</v>
       </c>
       <c r="F125">
-        <v>-0.00593617232516408</v>
+        <v>0.165923535823822</v>
       </c>
       <c r="G125">
-        <v>0.02601788751780987</v>
+        <v>0.1956327259540558</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3722,22 +3722,22 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>0.09552734345197678</v>
+        <v>-0.3643823266029358</v>
       </c>
       <c r="C126">
-        <v>0.03453272953629494</v>
+        <v>-0.4239953458309174</v>
       </c>
       <c r="D126">
         <v>0.01385040488094091</v>
       </c>
       <c r="E126">
-        <v>-0.9802999496459961</v>
+        <v>-0.9712534546852112</v>
       </c>
       <c r="F126">
-        <v>-0.006166554987430573</v>
+        <v>-0.009985870681703091</v>
       </c>
       <c r="G126">
-        <v>-0.576635479927063</v>
+        <v>-0.888243556022644</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3745,22 +3745,22 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>-0.1259008795022964</v>
+        <v>-0.585391104221344</v>
       </c>
       <c r="C127">
-        <v>-0.433199405670166</v>
+        <v>-0.687100887298584</v>
       </c>
       <c r="D127">
         <v>0.07607804238796234</v>
       </c>
       <c r="E127">
-        <v>-0.9303639531135559</v>
+        <v>-0.8581562042236328</v>
       </c>
       <c r="F127">
-        <v>-0.0003435839898884296</v>
+        <v>0.04139484092593193</v>
       </c>
       <c r="G127">
-        <v>-0.7925872206687927</v>
+        <v>-0.9144371747970581</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3768,22 +3768,22 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>0.06971698254346848</v>
+        <v>-0.4426668882369995</v>
       </c>
       <c r="C128">
-        <v>-0.4497626125812531</v>
+        <v>-0.8241918087005615</v>
       </c>
       <c r="D128">
         <v>0.03927205502986908</v>
       </c>
       <c r="E128">
-        <v>-0.962776780128479</v>
+        <v>-0.9202470779418945</v>
       </c>
       <c r="F128">
-        <v>0.01824347861111164</v>
+        <v>0.0271051786839962</v>
       </c>
       <c r="G128">
-        <v>0.91159588098526</v>
+        <v>-0.9293227195739746</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3791,22 +3791,22 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>0.2702292501926422</v>
+        <v>-0.195137083530426</v>
       </c>
       <c r="C129">
-        <v>0.2760631740093231</v>
+        <v>-0.4472408294677734</v>
       </c>
       <c r="D129">
         <v>-0.1553581058979034</v>
       </c>
       <c r="E129">
-        <v>-0.1519333124160767</v>
+        <v>-0.9791603088378906</v>
       </c>
       <c r="F129">
-        <v>0.02249131910502911</v>
+        <v>0.06396589428186417</v>
       </c>
       <c r="G129">
-        <v>-0.7477235198020935</v>
+        <v>-0.8644179701805115</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3814,22 +3814,22 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>-0.07717006653547287</v>
+        <v>-0.2952048778533936</v>
       </c>
       <c r="C130">
-        <v>0.5150648355484009</v>
+        <v>-0.2268115729093552</v>
       </c>
       <c r="D130">
         <v>0.1456242501735687</v>
       </c>
       <c r="E130">
-        <v>-0.9390866160392761</v>
+        <v>-0.9697768688201904</v>
       </c>
       <c r="F130">
-        <v>-0.03759227693080902</v>
+        <v>0.01360463816672564</v>
       </c>
       <c r="G130">
-        <v>-0.2700289189815521</v>
+        <v>-0.9492337107658386</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3837,22 +3837,22 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>0.1056789755821228</v>
+        <v>-0.01205745618790388</v>
       </c>
       <c r="C131">
-        <v>-0.9635457992553711</v>
+        <v>-0.8665860295295715</v>
       </c>
       <c r="D131">
         <v>-0.01691167987883091</v>
       </c>
       <c r="E131">
-        <v>-0.9988138675689697</v>
+        <v>-0.9820847511291504</v>
       </c>
       <c r="F131">
-        <v>-0.006638217717409134</v>
+        <v>0.03894798085093498</v>
       </c>
       <c r="G131">
-        <v>-0.9243074655532837</v>
+        <v>-0.9745551943778992</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3860,22 +3860,22 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>0.07701747864484787</v>
+        <v>-0.2398387938737869</v>
       </c>
       <c r="C132">
-        <v>-0.119694285094738</v>
+        <v>-0.8156892061233521</v>
       </c>
       <c r="D132">
         <v>-0.1031007096171379</v>
       </c>
       <c r="E132">
-        <v>-0.1182551607489586</v>
+        <v>-0.4487824440002441</v>
       </c>
       <c r="F132">
-        <v>-0.006815518718212843</v>
+        <v>0.04141780361533165</v>
       </c>
       <c r="G132">
-        <v>-0.7160730957984924</v>
+        <v>0.2444902658462524</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3883,22 +3883,22 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>-0.1359665989875793</v>
+        <v>-0.2639352977275848</v>
       </c>
       <c r="C133">
-        <v>-0.8207018971443176</v>
+        <v>-0.7698156237602234</v>
       </c>
       <c r="D133">
         <v>-0.006352945696562529</v>
       </c>
       <c r="E133">
-        <v>-0.984563946723938</v>
+        <v>-0.4268540143966675</v>
       </c>
       <c r="F133">
-        <v>-0.005388655699789524</v>
+        <v>0.02858619205653667</v>
       </c>
       <c r="G133">
-        <v>-0.4374058544635773</v>
+        <v>-0.7566240429878235</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3906,22 +3906,22 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>0.09098591655492783</v>
+        <v>-0.7422137260437012</v>
       </c>
       <c r="C134">
-        <v>-0.1719539612531662</v>
+        <v>-0.3463012874126434</v>
       </c>
       <c r="D134">
         <v>0.003470372408628464</v>
       </c>
       <c r="E134">
-        <v>-0.7996397018432617</v>
+        <v>0.378213107585907</v>
       </c>
       <c r="F134">
-        <v>0.04340776801109314</v>
+        <v>0.04929744824767113</v>
       </c>
       <c r="G134">
-        <v>0.7890831828117371</v>
+        <v>0.1555194109678268</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3929,22 +3929,22 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>0.1230873242020607</v>
+        <v>-0.7818644046783447</v>
       </c>
       <c r="C135">
-        <v>-0.8469343781471252</v>
+        <v>-0.8556920886039734</v>
       </c>
       <c r="D135">
         <v>0.08229725062847137</v>
       </c>
       <c r="E135">
-        <v>-0.9966615438461304</v>
+        <v>-0.9860680103302002</v>
       </c>
       <c r="F135">
-        <v>0.08189567923545837</v>
+        <v>0.007471553981304169</v>
       </c>
       <c r="G135">
-        <v>-0.9029055833816528</v>
+        <v>-0.9392798542976379</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3952,22 +3952,22 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>0.07377729564905167</v>
+        <v>-0.0790560320019722</v>
       </c>
       <c r="C136">
-        <v>0.5193066000938416</v>
+        <v>-0.4717240333557129</v>
       </c>
       <c r="D136">
         <v>0.03481919690966606</v>
       </c>
       <c r="E136">
-        <v>-0.8555403351783752</v>
+        <v>-0.8195508718490601</v>
       </c>
       <c r="F136">
-        <v>-0.04605524241924286</v>
+        <v>-0.04204880446195602</v>
       </c>
       <c r="G136">
-        <v>-0.8590609431266785</v>
+        <v>-0.2156109809875488</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -3975,22 +3975,22 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>0.003947800491005182</v>
+        <v>-0.4280498027801514</v>
       </c>
       <c r="C137">
-        <v>-0.3115902543067932</v>
+        <v>-0.7513765692710876</v>
       </c>
       <c r="D137">
         <v>0.01067364308983088</v>
       </c>
       <c r="E137">
-        <v>-0.7137587666511536</v>
+        <v>-0.9616966247558594</v>
       </c>
       <c r="F137">
-        <v>0.00317887426353991</v>
+        <v>0.009296378120779991</v>
       </c>
       <c r="G137">
-        <v>-0.9390555024147034</v>
+        <v>-0.4771688878536224</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -3998,22 +3998,22 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>-0.01285531558096409</v>
+        <v>-0.8463138341903687</v>
       </c>
       <c r="C138">
-        <v>-0.64324951171875</v>
+        <v>-0.9700772166252136</v>
       </c>
       <c r="D138">
         <v>-0.02489490993320942</v>
       </c>
       <c r="E138">
-        <v>-0.9810234904289246</v>
+        <v>0.5057421922683716</v>
       </c>
       <c r="F138">
-        <v>-0.05977893620729446</v>
+        <v>0.032677061855793</v>
       </c>
       <c r="G138">
-        <v>-0.9719235897064209</v>
+        <v>0.3414057195186615</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -4021,22 +4021,22 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>0.1568548977375031</v>
+        <v>-0.5170331001281738</v>
       </c>
       <c r="C139">
-        <v>0.6426762938499451</v>
+        <v>-0.6746819019317627</v>
       </c>
       <c r="D139">
         <v>0.09738272428512573</v>
       </c>
       <c r="E139">
-        <v>-0.6521057486534119</v>
+        <v>-0.6843129396438599</v>
       </c>
       <c r="F139">
-        <v>0.01200830191373825</v>
+        <v>0.02764411643147469</v>
       </c>
       <c r="G139">
-        <v>-0.9735549688339233</v>
+        <v>-0.03878914564847946</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -4044,22 +4044,22 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>-0.01247531361877918</v>
+        <v>-0.4399619102478027</v>
       </c>
       <c r="C140">
-        <v>0.1737743616104126</v>
+        <v>-0.8333253264427185</v>
       </c>
       <c r="D140">
         <v>0.05457809567451477</v>
       </c>
       <c r="E140">
-        <v>-0.7258781790733337</v>
+        <v>-0.9141754508018494</v>
       </c>
       <c r="F140">
-        <v>-0.01211346592754126</v>
+        <v>0.09881218522787094</v>
       </c>
       <c r="G140">
-        <v>-0.9389707446098328</v>
+        <v>-0.9287212491035461</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -4067,22 +4067,22 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>0.3310484290122986</v>
+        <v>-0.664857029914856</v>
       </c>
       <c r="C141">
-        <v>-0.6398292779922485</v>
+        <v>-0.5202570557594299</v>
       </c>
       <c r="D141">
         <v>0.03935513645410538</v>
       </c>
       <c r="E141">
-        <v>-0.9599238038063049</v>
+        <v>-0.9994841814041138</v>
       </c>
       <c r="F141">
-        <v>0.06644971668720245</v>
+        <v>-0.0685964971780777</v>
       </c>
       <c r="G141">
-        <v>0.6773750185966492</v>
+        <v>-0.9993636608123779</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -4090,22 +4090,22 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>0.1809795498847961</v>
+        <v>-0.5516170263290405</v>
       </c>
       <c r="C142">
-        <v>0.1010737195611</v>
+        <v>-0.9503968954086304</v>
       </c>
       <c r="D142">
         <v>-0.06708797067403793</v>
       </c>
       <c r="E142">
-        <v>-0.9839667677879333</v>
+        <v>-0.994046151638031</v>
       </c>
       <c r="F142">
-        <v>-0.02401226200163364</v>
+        <v>-0.1005102694034576</v>
       </c>
       <c r="G142">
-        <v>-0.8284235000610352</v>
+        <v>-0.9621206521987915</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -4113,22 +4113,22 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>-0.07388729602098465</v>
+        <v>0.3683362305164337</v>
       </c>
       <c r="C143">
-        <v>0.1645137220621109</v>
+        <v>0.3557892441749573</v>
       </c>
       <c r="D143">
         <v>0.04818234220147133</v>
       </c>
       <c r="E143">
-        <v>-0.9109460711479187</v>
+        <v>-0.8955475687980652</v>
       </c>
       <c r="F143">
-        <v>-0.02118578739464283</v>
+        <v>-0.04707549884915352</v>
       </c>
       <c r="G143">
-        <v>-0.6138535737991333</v>
+        <v>-0.9655057191848755</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -4136,22 +4136,22 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>0.001543424325063825</v>
+        <v>-0.1832160651683807</v>
       </c>
       <c r="C144">
-        <v>-0.284855842590332</v>
+        <v>-0.9147796034812927</v>
       </c>
       <c r="D144">
         <v>0.1414187103509903</v>
       </c>
       <c r="E144">
-        <v>-0.9998430013656616</v>
+        <v>-0.8812951445579529</v>
       </c>
       <c r="F144">
-        <v>0.03746149688959122</v>
+        <v>-0.07149498909711838</v>
       </c>
       <c r="G144">
-        <v>0.494472861289978</v>
+        <v>-0.659781277179718</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -4159,22 +4159,22 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>-0.1581306457519531</v>
+        <v>-0.2198426574468613</v>
       </c>
       <c r="C145">
-        <v>-0.6942527890205383</v>
+        <v>-0.9360929727554321</v>
       </c>
       <c r="D145">
         <v>-0.04850566759705544</v>
       </c>
       <c r="E145">
-        <v>-0.9400984644889832</v>
+        <v>-0.9928490519523621</v>
       </c>
       <c r="F145">
-        <v>-0.0375918447971344</v>
+        <v>-0.1352222710847855</v>
       </c>
       <c r="G145">
-        <v>-0.7664948701858521</v>
+        <v>-0.9882159233093262</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -4182,22 +4182,22 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>0.1918644458055496</v>
+        <v>-0.3037092089653015</v>
       </c>
       <c r="C146">
-        <v>-0.4451876580715179</v>
+        <v>-0.6805959343910217</v>
       </c>
       <c r="D146">
         <v>0.03549801930785179</v>
       </c>
       <c r="E146">
-        <v>-0.9846748113632202</v>
+        <v>0.1275187581777573</v>
       </c>
       <c r="F146">
-        <v>0.01433489378541708</v>
+        <v>-0.03216149657964706</v>
       </c>
       <c r="G146">
-        <v>-0.4538972675800323</v>
+        <v>-0.2733826041221619</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -4205,22 +4205,22 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>0.005460433196276426</v>
+        <v>-0.07314053922891617</v>
       </c>
       <c r="C147">
-        <v>0.07882419973611832</v>
+        <v>0.1049581915140152</v>
       </c>
       <c r="D147">
         <v>0.07950207591056824</v>
       </c>
       <c r="E147">
-        <v>-0.9679996967315674</v>
+        <v>-0.996720552444458</v>
       </c>
       <c r="F147">
-        <v>-0.03207681700587273</v>
+        <v>-0.09773352742195129</v>
       </c>
       <c r="G147">
-        <v>-0.6691401600837708</v>
+        <v>-0.9951809048652649</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -4228,22 +4228,22 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>-0.009174126200377941</v>
+        <v>-0.5968519449234009</v>
       </c>
       <c r="C148">
-        <v>0.04794313013553619</v>
+        <v>-0.5844030976295471</v>
       </c>
       <c r="D148">
         <v>0.04609322920441628</v>
       </c>
       <c r="E148">
-        <v>-0.8903407454490662</v>
+        <v>-0.9493703246116638</v>
       </c>
       <c r="F148">
-        <v>0.01523424405604601</v>
+        <v>0.07644741237163544</v>
       </c>
       <c r="G148">
-        <v>-0.8700944185256958</v>
+        <v>-0.9532349705696106</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -4251,22 +4251,22 @@
         <v>147</v>
       </c>
       <c r="B149">
-        <v>-0.1687502413988113</v>
+        <v>-0.07842059433460236</v>
       </c>
       <c r="C149">
-        <v>0.04331400990486145</v>
+        <v>-0.5215400457382202</v>
       </c>
       <c r="D149">
         <v>0.04515611380338669</v>
       </c>
       <c r="E149">
-        <v>-0.8501381278038025</v>
+        <v>-0.7851879000663757</v>
       </c>
       <c r="F149">
-        <v>-0.03696342557668686</v>
+        <v>-0.003382339375093579</v>
       </c>
       <c r="G149">
-        <v>-0.6934669017791748</v>
+        <v>-0.7567638754844666</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -4274,22 +4274,22 @@
         <v>148</v>
       </c>
       <c r="B150">
-        <v>0.04247300326824188</v>
+        <v>-0.3154294788837433</v>
       </c>
       <c r="C150">
-        <v>0.01484467927366495</v>
+        <v>-0.7796546220779419</v>
       </c>
       <c r="D150">
         <v>0.05780215933918953</v>
       </c>
       <c r="E150">
-        <v>-0.8652666211128235</v>
+        <v>0.433720588684082</v>
       </c>
       <c r="F150">
-        <v>-0.06231579557061195</v>
+        <v>-0.03452889993786812</v>
       </c>
       <c r="G150">
-        <v>-0.2843629121780396</v>
+        <v>0.420377790927887</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -4297,22 +4297,22 @@
         <v>149</v>
       </c>
       <c r="B151">
-        <v>0.1086578220129013</v>
+        <v>-0.4564280211925507</v>
       </c>
       <c r="C151">
-        <v>0.4579405188560486</v>
+        <v>-0.7157658338546753</v>
       </c>
       <c r="D151">
         <v>0.01813386753201485</v>
       </c>
       <c r="E151">
-        <v>-0.9052119255065918</v>
+        <v>-0.9335408210754395</v>
       </c>
       <c r="F151">
-        <v>-0.04157527163624763</v>
+        <v>0.06778275966644287</v>
       </c>
       <c r="G151">
-        <v>-0.7695709466934204</v>
+        <v>-0.875805675983429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>